<commit_message>
Actualizado taller Robot Delta
</commit_message>
<xml_diff>
--- a/03a_Delta/04_Otros/08_Taller_RobotDelta/Estudiantes.xlsx
+++ b/03a_Delta/04_Otros/08_Taller_RobotDelta/Estudiantes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAG\Documents\MecanismosPythonUPB\03a_Delta\04_Otros\08_Taller_RobotDelta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\000092114\Documents\MecanismosPythonUPB\03a_Delta\04_Otros\08_Taller_RobotDelta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B263DA89-EB8A-42A2-B737-67CDC9410E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E01387C-1397-4761-AFB5-6CDE464B4413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B8024D5-D2CD-4F16-AC49-88DDC0870749}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -38,66 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t>AGUDELO FERIZ, VALENTINA</t>
-  </si>
-  <si>
-    <t>CHACON GALLEGO, DAVID</t>
-  </si>
-  <si>
-    <t>GALLEGO ALZATE, DANIEL</t>
-  </si>
-  <si>
-    <t>MADRID RANGEL, JUAN M.</t>
-  </si>
-  <si>
-    <t>ORTEGA CASTAÑO, SEBASTIAN</t>
-  </si>
-  <si>
-    <t>OSPINA JARAMILLO, PABLO</t>
-  </si>
-  <si>
-    <t>REGALADO CHICAIZA, SEBASTIAN M.</t>
-  </si>
-  <si>
-    <t>RINCON GUTIERREZ, DANIEL</t>
-  </si>
-  <si>
-    <t>SIERRA GUERRERO, JOSE F.</t>
-  </si>
-  <si>
-    <t>TAMAYO AGUDELO, DAVID</t>
-  </si>
-  <si>
-    <t>VAHOS SERNA, JULIO C.</t>
-  </si>
-  <si>
-    <t>VEGA RODRIGUEZ, SANTIAGO</t>
-  </si>
-  <si>
-    <t>WHITE RESTREPO, TOMAS</t>
-  </si>
-  <si>
-    <t>ZULUAGA ARISTIZABAL, ANDRES</t>
-  </si>
-  <si>
-    <t>CALAO JIMENEZ, VALENTINA</t>
-  </si>
-  <si>
-    <t>JAIME ALZATE, CRISTIAN CAMILO</t>
-  </si>
-  <si>
-    <t>PEREZ DE LOS RIOS, LEONARDO</t>
-  </si>
-  <si>
-    <t>ROMERO CASTILLO, SARA C.</t>
-  </si>
-  <si>
-    <t>SILVA RIOS, VALERIA</t>
-  </si>
-  <si>
-    <t>VANEGAS DIAZ, SOFIA</t>
-  </si>
-  <si>
     <t>Est</t>
   </si>
   <si>
@@ -105,6 +34,66 @@
   </si>
   <si>
     <t>grupo</t>
+  </si>
+  <si>
+    <t>BUITRAGO MEDINA, JUAN C.</t>
+  </si>
+  <si>
+    <t>HERNANDEZ JIMENEZ, ANA M.</t>
+  </si>
+  <si>
+    <t>JIMENEZ GIRALDO, JUAN P.</t>
+  </si>
+  <si>
+    <t>MARIN ARROYAVE, JUAN J.</t>
+  </si>
+  <si>
+    <t>MARIN ZABALA, STEPHANIA</t>
+  </si>
+  <si>
+    <t>MURIEL AGUDELO, SARA P.</t>
+  </si>
+  <si>
+    <t>PEÑARANDA BOTELLO, DEIMER L.</t>
+  </si>
+  <si>
+    <t>ROJAS VASQUEZ, JUAN C.</t>
+  </si>
+  <si>
+    <t>SOTO JARAMILLO, JUAN J.</t>
+  </si>
+  <si>
+    <t>TOBON PEÑA, MARIA J.</t>
+  </si>
+  <si>
+    <t>VALERA MASS, JOSE A.</t>
+  </si>
+  <si>
+    <t>CASTRO AGUDELO, SAMUEL E.</t>
+  </si>
+  <si>
+    <t>DE LA CRUZ VERGARA, ELBA LUCIA</t>
+  </si>
+  <si>
+    <t>GUISAO LOPEZ, JULIAN</t>
+  </si>
+  <si>
+    <t>HERRERA ESTRADA, SANTIAGO</t>
+  </si>
+  <si>
+    <t>MEJIA TAMAYO , SANTIAGO</t>
+  </si>
+  <si>
+    <t>MENESES MONTOYA, SANTIAGO</t>
+  </si>
+  <si>
+    <t>RAMIREZ VELEZ, CAMILO</t>
+  </si>
+  <si>
+    <t>TABARES BROWN, TOMAS</t>
+  </si>
+  <si>
+    <t>VASQUEZ MONTOYA, VALERIA</t>
   </si>
 </sst>
 </file>
@@ -686,26 +675,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945C758E-2908-43D8-B361-B800697AD4B6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -714,9 +703,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -725,9 +714,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
@@ -736,9 +725,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -747,9 +736,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6">
         <v>5</v>
@@ -758,9 +747,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
@@ -769,9 +758,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5">
         <v>7</v>
@@ -780,9 +769,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6">
         <v>8</v>
@@ -791,9 +780,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7">
         <v>9</v>
@@ -802,9 +791,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="6">
         <v>10</v>
@@ -813,9 +802,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12" s="7">
         <v>11</v>
@@ -824,9 +813,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6">
         <v>12</v>
@@ -835,31 +824,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14" s="8">
         <v>13</v>
       </c>
       <c r="C14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15" s="9">
         <v>14</v>
       </c>
       <c r="C15" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" s="10">
         <v>15</v>
@@ -868,9 +857,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" s="10">
         <v>16</v>
@@ -879,31 +868,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10">
         <v>17</v>
       </c>
       <c r="C18" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" s="10">
         <v>18</v>
       </c>
       <c r="C19" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" s="10">
         <v>19</v>
@@ -912,15 +901,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="10">
         <v>20</v>
       </c>
       <c r="C21" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>